<commit_message>
Ran model for Clavigralla species; organized repo files
</commit_message>
<xml_diff>
--- a/Insect database.xlsx
+++ b/Insect database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11002"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A3313F36-54B0-9B46-A479-F1F7071249AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B124E1-3750-FA49-A84B-120D7BEBFEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="17500"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data base" sheetId="1" r:id="rId1"/>
@@ -737,7 +737,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1627,11 +1627,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1710,7 +1710,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K2" s="1"/>
     </row>
@@ -2892,7 +2892,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
@@ -3994,7 +3994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">

</xml_diff>

<commit_message>
Minor changes to computational pipeline
</commit_message>
<xml_diff>
--- a/Insect database.xlsx
+++ b/Insect database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B124E1-3750-FA49-A84B-120D7BEBFEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55760AF-F992-E34A-8CB1-F9F02549896D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="28780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="230">
   <si>
     <t>Species</t>
   </si>
@@ -732,6 +732,9 @@
   </si>
   <si>
     <t>Perdikis &amp; Lykouressis 1999</t>
+  </si>
+  <si>
+    <t>Also has development and juvenile mortality data</t>
   </si>
 </sst>
 </file>
@@ -1631,7 +1634,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1813,7 +1816,9 @@
       <c r="J5" s="1">
         <v>8</v>
       </c>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">

</xml_diff>

<commit_message>
Added two insects from Japan and updated fitted estimates of r
</commit_message>
<xml_diff>
--- a/Insect database.xlsx
+++ b/Insect database.xlsx
@@ -1,28 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11006"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA12E41-9EA0-0244-BB3E-E0A478041DE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB19E591-681A-6E44-B78C-69082BB94C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35620" yWindow="3580" windowWidth="28780" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data base" sheetId="1" r:id="rId1"/>
     <sheet name="New refs" sheetId="2" r:id="rId2"/>
     <sheet name="Not included" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="233">
   <si>
     <t>Species</t>
   </si>
@@ -735,6 +745,15 @@
   </si>
   <si>
     <t>China Langfang</t>
+  </si>
+  <si>
+    <t>Citrus unshiu</t>
+  </si>
+  <si>
+    <t>Citrus aurantium</t>
+  </si>
+  <si>
+    <t>Not used because only 4 temperatures for most traits</t>
   </si>
 </sst>
 </file>
@@ -1633,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2225,6 +2244,9 @@
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C18" t="s">
+        <v>230</v>
+      </c>
       <c r="D18" s="1">
         <v>35.380000000000003</v>
       </c>
@@ -2235,7 +2257,7 @@
         <v>57</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>53</v>
@@ -2245,6 +2267,9 @@
       </c>
       <c r="J18" s="1">
         <v>4</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -2254,6 +2279,9 @@
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C19" t="s">
+        <v>231</v>
+      </c>
       <c r="D19" s="1">
         <v>35.380000000000003</v>
       </c>
@@ -2264,7 +2292,7 @@
         <v>57</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>53</v>
@@ -2283,6 +2311,9 @@
       <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C20" t="s">
+        <v>230</v>
+      </c>
       <c r="D20" s="1">
         <v>35.380000000000003</v>
       </c>
@@ -2293,7 +2324,7 @@
         <v>57</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>53</v>
@@ -2312,6 +2343,9 @@
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C21" t="s">
+        <v>230</v>
+      </c>
       <c r="D21" s="1">
         <v>35.380000000000003</v>
       </c>
@@ -2322,7 +2356,7 @@
         <v>57</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>53</v>
@@ -2332,6 +2366,9 @@
       </c>
       <c r="J21" s="1">
         <v>5</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Have now fit life history trait responses for 30 insects
</commit_message>
<xml_diff>
--- a/Insect database.xlsx
+++ b/Insect database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE684A9-A2CC-BC43-A228-E4B58BF2C8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39630C74-B5A0-5F4B-BECF-F2ABA50E97E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28780" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="268">
   <si>
     <t>Species</t>
   </si>
@@ -197,9 +197,6 @@
   </si>
   <si>
     <t>Aphis gossypii</t>
-  </si>
-  <si>
-    <t>Not yet</t>
   </si>
   <si>
     <t>Acyrthosiphon pisum</t>
@@ -850,6 +847,18 @@
   </si>
   <si>
     <t>sycamore</t>
+  </si>
+  <si>
+    <t>Not used because unimodal function cannot be fit for development</t>
+  </si>
+  <si>
+    <t>Amarasekare</t>
+  </si>
+  <si>
+    <t>Murgantia histrionica</t>
+  </si>
+  <si>
+    <t>No data on r or R0</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1069,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1240,6 +1249,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1401,7 +1416,7 @@
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1416,6 +1431,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1773,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1822,7 +1838,7 @@
         <v>30</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>31</v>
@@ -1860,7 +1876,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K2" s="10">
         <v>8</v>
@@ -1895,13 +1911,13 @@
         <v>5</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K3" s="10">
         <v>8</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1933,13 +1949,13 @@
         <v>5</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K4" s="10">
         <v>8</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1971,7 +1987,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K5" s="10">
         <v>9</v>
@@ -2006,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K6" s="10">
         <v>6</v>
@@ -2044,7 +2060,7 @@
         <v>5</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K7" s="10">
         <v>6</v>
@@ -2058,7 +2074,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>25</v>
@@ -2082,7 +2098,7 @@
         <v>5</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K8" s="10">
         <v>6</v>
@@ -2120,7 +2136,7 @@
         <v>5</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K9" s="10">
         <v>6</v>
@@ -2158,7 +2174,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K10" s="10">
         <v>5</v>
@@ -2193,7 +2209,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K11" s="10">
         <v>5</v>
@@ -2226,7 +2242,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K12" s="10">
         <v>5</v>
@@ -2258,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K13" s="10">
         <v>5</v>
@@ -2290,7 +2306,7 @@
         <v>8</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K14" s="10">
         <v>5</v>
@@ -2301,7 +2317,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D15" s="10">
         <v>33.619999999999997</v>
@@ -2310,9 +2326,9 @@
         <v>133.66999999999999</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="G15" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H15" s="10" t="s">
@@ -2322,7 +2338,7 @@
         <v>5</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K15" s="10">
         <v>6</v>
@@ -2336,7 +2352,7 @@
         <v>45</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D16" s="10">
         <v>33.42</v>
@@ -2347,7 +2363,7 @@
       <c r="F16" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H16" s="10" t="s">
@@ -2357,7 +2373,7 @@
         <v>5</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K16" s="10">
         <v>7</v>
@@ -2371,10 +2387,10 @@
         <v>51</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D17" s="10">
         <v>35.380000000000003</v>
@@ -2395,7 +2411,7 @@
         <v>8</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K17" s="10">
         <v>5</v>
@@ -2406,10 +2422,10 @@
         <v>51</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D18" s="10">
         <v>35.380000000000003</v>
@@ -2430,7 +2446,7 @@
         <v>8</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K18" s="10">
         <v>7</v>
@@ -2441,10 +2457,10 @@
         <v>53</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D19" s="10">
         <v>35.380000000000003</v>
@@ -2465,7 +2481,7 @@
         <v>8</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" s="10">
         <v>6</v>
@@ -2476,10 +2492,10 @@
         <v>54</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D20" s="10">
         <v>35.380000000000003</v>
@@ -2490,7 +2506,7 @@
       <c r="F20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H20" s="10" t="s">
@@ -2500,7 +2516,7 @@
         <v>8</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K20" s="10">
         <v>5</v>
@@ -2511,13 +2527,13 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>57</v>
       </c>
       <c r="D21" s="10">
         <v>54.02</v>
@@ -2526,7 +2542,7 @@
         <v>-0.97</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>38</v>
@@ -2538,24 +2554,24 @@
         <v>8</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K21" s="10">
         <v>5</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D22" s="10">
         <v>25.47</v>
@@ -2564,7 +2580,7 @@
         <v>-80.48</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>38</v>
@@ -2576,24 +2592,24 @@
         <v>8</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K22" s="10">
         <v>6</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D23" s="10">
         <v>26.14</v>
@@ -2602,7 +2618,7 @@
         <v>-81.790000000000006</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>38</v>
@@ -2614,7 +2630,7 @@
         <v>8</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K23" s="10">
         <v>6</v>
@@ -2622,10 +2638,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>23</v>
@@ -2637,7 +2653,7 @@
         <v>-80.45</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" s="10" t="s">
         <v>38</v>
@@ -2649,7 +2665,7 @@
         <v>8</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K24" s="10">
         <v>7</v>
@@ -2657,13 +2673,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D25" s="10">
         <v>26.24</v>
@@ -2672,7 +2688,7 @@
         <v>-80.12</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>38</v>
@@ -2684,7 +2700,7 @@
         <v>8</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K25" s="10">
         <v>7</v>
@@ -2692,13 +2708,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D26" s="11">
         <v>-30.9</v>
@@ -2707,7 +2723,7 @@
         <v>115.78</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>38</v>
@@ -2719,7 +2735,7 @@
         <v>8</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K26" s="10">
         <v>7</v>
@@ -2730,7 +2746,7 @@
         <v>54</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D27" s="10">
         <v>33.69</v>
@@ -2739,10 +2755,10 @@
         <v>-101.8</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="G27" s="10" t="s">
-        <v>55</v>
+        <v>72</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>48</v>
@@ -2751,21 +2767,24 @@
         <v>8</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K27" s="10">
         <v>6</v>
       </c>
+      <c r="L27" s="10" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D28" s="10">
         <v>52.62</v>
@@ -2774,9 +2793,9 @@
         <v>1.24</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H28" s="10" t="s">
@@ -2786,24 +2805,24 @@
         <v>8</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K28" s="10">
         <v>5</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D29" s="10">
         <v>52.62</v>
@@ -2812,9 +2831,9 @@
         <v>1.24</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H29" s="10" t="s">
@@ -2824,13 +2843,13 @@
         <v>8</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K29" s="10">
         <v>5</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2838,7 +2857,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="10">
         <v>42.81</v>
@@ -2847,10 +2866,10 @@
         <v>-82.23</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H30" s="10" t="s">
         <v>6</v>
@@ -2859,7 +2878,7 @@
         <v>8</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K30" s="10">
         <v>6</v>
@@ -2870,7 +2889,7 @@
         <v>34</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="10">
         <v>42.81</v>
@@ -2879,10 +2898,10 @@
         <v>-82.23</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>6</v>
@@ -2891,7 +2910,7 @@
         <v>8</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K31" s="10">
         <v>6</v>
@@ -2899,10 +2918,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D32" s="10">
         <v>-35.270000000000003</v>
@@ -2911,10 +2930,10 @@
         <v>149.11000000000001</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H32" s="10" t="s">
         <v>48</v>
@@ -2923,7 +2942,7 @@
         <v>8</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K32" s="10">
         <v>6</v>
@@ -2934,10 +2953,10 @@
         <v>54</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D33" s="10">
         <v>35.75</v>
@@ -2946,10 +2965,10 @@
         <v>51.17</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" s="10" t="s">
-        <v>55</v>
+        <v>76</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="H33" s="10" t="s">
         <v>48</v>
@@ -2958,10 +2977,13 @@
         <v>8</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K33" s="10">
         <v>6</v>
+      </c>
+      <c r="L33" s="10" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
@@ -2969,7 +2991,7 @@
         <v>54</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>25</v>
@@ -2981,10 +3003,10 @@
         <v>114.22</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>6</v>
@@ -2993,24 +3015,21 @@
         <v>8</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K34" s="10">
         <v>6</v>
       </c>
-      <c r="L34" s="10" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D35" s="10">
         <v>42.42</v>
@@ -3019,10 +3038,10 @@
         <v>-76.53</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>6</v>
@@ -3031,7 +3050,7 @@
         <v>8</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K35" s="10">
         <v>6</v>
@@ -3039,10 +3058,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D36" s="10">
         <v>38.93</v>
@@ -3051,10 +3070,10 @@
         <v>-92.34</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>6</v>
@@ -3063,7 +3082,7 @@
         <v>8</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K36" s="10">
         <v>7</v>
@@ -3074,7 +3093,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D37" s="10">
         <v>38.93</v>
@@ -3083,10 +3102,10 @@
         <v>-92.34</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>6</v>
@@ -3095,7 +3114,7 @@
         <v>8</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K37" s="10">
         <v>7</v>
@@ -3103,10 +3122,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D38" s="10">
         <v>38.93</v>
@@ -3115,10 +3134,10 @@
         <v>-92.34</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>6</v>
@@ -3127,7 +3146,7 @@
         <v>8</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K38" s="10">
         <v>7</v>
@@ -3159,10 +3178,10 @@
         <v>29</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>85</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -3170,13 +3189,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>54</v>
@@ -3184,13 +3203,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>34</v>
@@ -3198,83 +3217,83 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>27</v>
@@ -3282,13 +3301,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>27</v>
@@ -3296,326 +3315,326 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>257</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>116</v>
-      </c>
       <c r="D25" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>54</v>
@@ -3623,13 +3642,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>54</v>
@@ -3637,13 +3656,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>54</v>
@@ -3651,13 +3670,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>54</v>
@@ -3665,27 +3684,27 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>129</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>54</v>
@@ -3693,41 +3712,41 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>54</v>
@@ -3735,13 +3754,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>54</v>
@@ -3749,27 +3768,27 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>138</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>54</v>
@@ -3777,25 +3796,25 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D47" s="7" t="s">
         <v>54</v>
@@ -3803,13 +3822,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>27</v>
@@ -3817,13 +3836,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>27</v>
@@ -3831,13 +3850,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>27</v>
@@ -3845,13 +3864,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>27</v>
@@ -3859,13 +3878,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>27</v>
@@ -3873,13 +3892,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>27</v>
@@ -3887,55 +3906,55 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>149</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>151</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>27</v>
@@ -3943,39 +3962,39 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>54</v>
@@ -3983,13 +4002,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>45</v>
@@ -3997,69 +4016,69 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D62" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>45</v>
@@ -4067,27 +4086,27 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>45</v>
@@ -4095,66 +4114,66 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>167</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D73" s="7" t="s">
         <v>32</v>
@@ -4162,111 +4181,111 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="3" t="s">
+      <c r="D74" s="7" t="s">
         <v>175</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D75" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="3" t="s">
+      <c r="D76" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>182</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D81" s="7" t="s">
         <v>32</v>
@@ -4274,66 +4293,66 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>241</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>245</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="7" t="s">
         <v>247</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D86" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -4343,15 +4362,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -4361,237 +4381,237 @@
         <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>85</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>265</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>189</v>
+      <c r="C2" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>190</v>
+        <v>266</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>19</v>
+        <v>192</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>188</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>198</v>
+        <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>20</v>
+        <v>197</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -4602,47 +4622,64 @@
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E18" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran DDE model for all insect species
</commit_message>
<xml_diff>
--- a/Insect database.xlsx
+++ b/Insect database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39630C74-B5A0-5F4B-BECF-F2ABA50E97E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA16E520-8B8F-5A41-B2ED-1F747D7715E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28780" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="269">
   <si>
     <t>Species</t>
   </si>
@@ -859,6 +859,9 @@
   </si>
   <si>
     <t>No data on r or R0</t>
+  </si>
+  <si>
+    <t>Extinct in previous climate</t>
   </si>
 </sst>
 </file>
@@ -1790,7 +1793,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2471,8 +2474,8 @@
       <c r="F19" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>38</v>
+      <c r="G19" s="14" t="s">
+        <v>39</v>
       </c>
       <c r="H19" s="10" t="s">
         <v>48</v>
@@ -2485,6 +2488,9 @@
       </c>
       <c r="K19" s="10">
         <v>6</v>
+      </c>
+      <c r="L19" s="10" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Working on model fits to census data
</commit_message>
<xml_diff>
--- a/Insect database.xlsx
+++ b/Insect database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA16E520-8B8F-5A41-B2ED-1F747D7715E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549D39A9-6D54-8D40-9FFE-E98B067B6D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28780" windowHeight="17260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="268">
   <si>
     <t>Species</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>Reference</t>
-  </si>
-  <si>
-    <t>Subfamily</t>
   </si>
   <si>
     <t>N_temps</t>
@@ -1792,8 +1789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1832,19 +1829,19 @@
         <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>3</v>
@@ -1867,10 +1864,10 @@
         <v>2.35</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>4</v>
@@ -1879,7 +1876,7 @@
         <v>5</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K2" s="10">
         <v>8</v>
@@ -1902,10 +1899,10 @@
         <v>2.35</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>4</v>
@@ -1914,13 +1911,13 @@
         <v>5</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K3" s="10">
         <v>8</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -1940,10 +1937,10 @@
         <v>3.9</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>4</v>
@@ -1952,13 +1949,13 @@
         <v>5</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K4" s="10">
         <v>8</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1978,10 +1975,10 @@
         <v>-1.5</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H5" s="10" t="s">
         <v>4</v>
@@ -1990,7 +1987,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K5" s="10">
         <v>9</v>
@@ -2013,10 +2010,10 @@
         <v>120.75</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="10" t="s">
         <v>6</v>
@@ -2025,13 +2022,13 @@
         <v>5</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K6" s="10">
         <v>6</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -2051,10 +2048,10 @@
         <v>120.75</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>6</v>
@@ -2063,13 +2060,13 @@
         <v>5</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K7" s="10">
         <v>6</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -2077,7 +2074,7 @@
         <v>20</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>25</v>
@@ -2089,10 +2086,10 @@
         <v>117.17</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>6</v>
@@ -2101,13 +2098,13 @@
         <v>5</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K8" s="10">
         <v>6</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2127,10 +2124,10 @@
         <v>114.42</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>6</v>
@@ -2139,24 +2136,24 @@
         <v>5</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K9" s="10">
         <v>6</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="10">
         <v>38.380000000000003</v>
@@ -2165,10 +2162,10 @@
         <v>23.14</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>7</v>
@@ -2177,7 +2174,7 @@
         <v>5</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K10" s="10">
         <v>5</v>
@@ -2185,13 +2182,13 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="10">
         <v>38.380000000000003</v>
@@ -2200,10 +2197,10 @@
         <v>23.14</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="10" t="s">
         <v>7</v>
@@ -2212,7 +2209,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K11" s="10">
         <v>5</v>
@@ -2233,10 +2230,10 @@
         <v>-44.98</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>4</v>
@@ -2245,7 +2242,7 @@
         <v>8</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K12" s="10">
         <v>5</v>
@@ -2265,10 +2262,10 @@
         <v>-44.98</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H13" s="10" t="s">
         <v>4</v>
@@ -2277,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K13" s="10">
         <v>5</v>
@@ -2297,10 +2294,10 @@
         <v>-44.98</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="10" t="s">
         <v>4</v>
@@ -2309,7 +2306,7 @@
         <v>8</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K14" s="10">
         <v>5</v>
@@ -2317,10 +2314,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D15" s="10">
         <v>33.619999999999997</v>
@@ -2329,33 +2326,33 @@
         <v>133.66999999999999</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>5</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K15" s="10">
         <v>6</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D16" s="10">
         <v>33.42</v>
@@ -2364,36 +2361,36 @@
         <v>-90.9</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>5</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K16" s="10">
         <v>7</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D17" s="10">
         <v>35.380000000000003</v>
@@ -2402,19 +2399,19 @@
         <v>140.07</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K17" s="10">
         <v>5</v>
@@ -2422,13 +2419,13 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D18" s="10">
         <v>35.380000000000003</v>
@@ -2437,19 +2434,19 @@
         <v>140.07</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K18" s="10">
         <v>7</v>
@@ -2457,13 +2454,13 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D19" s="10">
         <v>35.380000000000003</v>
@@ -2472,36 +2469,36 @@
         <v>140.07</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K19" s="10">
         <v>6</v>
       </c>
       <c r="L19" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D20" s="10">
         <v>35.380000000000003</v>
@@ -2510,36 +2507,36 @@
         <v>140.07</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K20" s="10">
         <v>5</v>
       </c>
       <c r="L20" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="D21" s="10">
         <v>54.02</v>
@@ -2548,10 +2545,10 @@
         <v>-0.97</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>6</v>
@@ -2560,24 +2557,24 @@
         <v>8</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K21" s="10">
         <v>5</v>
       </c>
       <c r="L21" s="10" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D22" s="10">
         <v>25.47</v>
@@ -2586,36 +2583,36 @@
         <v>-80.48</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H22" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K22" s="10">
         <v>6</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D23" s="10">
         <v>26.14</v>
@@ -2624,19 +2621,19 @@
         <v>-81.790000000000006</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K23" s="10">
         <v>6</v>
@@ -2644,10 +2641,10 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>23</v>
@@ -2659,19 +2656,19 @@
         <v>-80.45</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K24" s="10">
         <v>7</v>
@@ -2679,13 +2676,13 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D25" s="10">
         <v>26.24</v>
@@ -2694,19 +2691,19 @@
         <v>-80.12</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H25" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K25" s="10">
         <v>7</v>
@@ -2714,13 +2711,13 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D26" s="11">
         <v>-30.9</v>
@@ -2729,19 +2726,19 @@
         <v>115.78</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K26" s="10">
         <v>7</v>
@@ -2749,10 +2746,10 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D27" s="10">
         <v>33.69</v>
@@ -2761,36 +2758,36 @@
         <v>-101.8</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K27" s="10">
         <v>6</v>
       </c>
       <c r="L27" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D28" s="10">
         <v>52.62</v>
@@ -2799,10 +2796,10 @@
         <v>1.24</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G28" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H28" s="10" t="s">
         <v>6</v>
@@ -2811,24 +2808,24 @@
         <v>8</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K28" s="10">
         <v>5</v>
       </c>
       <c r="L28" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D29" s="10">
         <v>52.62</v>
@@ -2837,10 +2834,10 @@
         <v>1.24</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G29" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H29" s="10" t="s">
         <v>6</v>
@@ -2849,13 +2846,13 @@
         <v>8</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K29" s="10">
         <v>5</v>
       </c>
       <c r="L29" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2863,7 +2860,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D30" s="10">
         <v>42.81</v>
@@ -2872,10 +2869,10 @@
         <v>-82.23</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="10" t="s">
         <v>6</v>
@@ -2884,7 +2881,7 @@
         <v>8</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K30" s="10">
         <v>6</v>
@@ -2892,10 +2889,10 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D31" s="10">
         <v>42.81</v>
@@ -2904,10 +2901,10 @@
         <v>-82.23</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H31" s="10" t="s">
         <v>6</v>
@@ -2916,7 +2913,7 @@
         <v>8</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K31" s="10">
         <v>6</v>
@@ -2924,10 +2921,10 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D32" s="10">
         <v>-35.270000000000003</v>
@@ -2936,19 +2933,19 @@
         <v>149.11000000000001</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H32" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K32" s="10">
         <v>6</v>
@@ -2956,13 +2953,13 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D33" s="10">
         <v>35.75</v>
@@ -2971,33 +2968,33 @@
         <v>51.17</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H33" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>8</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K33" s="10">
         <v>6</v>
       </c>
       <c r="L33" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>25</v>
@@ -3009,10 +3006,10 @@
         <v>114.22</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H34" s="10" t="s">
         <v>6</v>
@@ -3021,7 +3018,7 @@
         <v>8</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K34" s="10">
         <v>6</v>
@@ -3029,13 +3026,13 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D35" s="10">
         <v>42.42</v>
@@ -3044,10 +3041,10 @@
         <v>-76.53</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H35" s="10" t="s">
         <v>6</v>
@@ -3056,7 +3053,7 @@
         <v>8</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K35" s="10">
         <v>6</v>
@@ -3064,10 +3061,10 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D36" s="10">
         <v>38.93</v>
@@ -3076,10 +3073,10 @@
         <v>-92.34</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H36" s="10" t="s">
         <v>6</v>
@@ -3088,7 +3085,7 @@
         <v>8</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K36" s="10">
         <v>7</v>
@@ -3096,10 +3093,10 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D37" s="10">
         <v>38.93</v>
@@ -3108,10 +3105,10 @@
         <v>-92.34</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H37" s="10" t="s">
         <v>6</v>
@@ -3120,7 +3117,7 @@
         <v>8</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K37" s="10">
         <v>7</v>
@@ -3128,10 +3125,10 @@
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D38" s="10">
         <v>38.93</v>
@@ -3140,10 +3137,10 @@
         <v>-92.34</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H38" s="10" t="s">
         <v>6</v>
@@ -3152,7 +3149,7 @@
         <v>8</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K38" s="10">
         <v>7</v>
@@ -3184,10 +3181,10 @@
         <v>29</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>0</v>
@@ -3195,111 +3192,111 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>90</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>27</v>
@@ -3307,13 +3304,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>27</v>
@@ -3321,520 +3318,520 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>99</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>256</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>115</v>
-      </c>
       <c r="D25" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>131</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="8" t="s">
+      <c r="D44" s="7" t="s">
         <v>137</v>
-      </c>
-      <c r="D44" s="7" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>27</v>
@@ -3842,13 +3839,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>27</v>
@@ -3856,13 +3853,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>27</v>
@@ -3870,13 +3867,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>27</v>
@@ -3884,13 +3881,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>27</v>
@@ -3898,13 +3895,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D53" s="7" t="s">
         <v>27</v>
@@ -3912,55 +3909,55 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>150</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D55" s="7" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D57" s="7" t="s">
         <v>27</v>
@@ -3968,397 +3965,397 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="D61" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D62" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D62" s="7" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D69" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="3" t="s">
+      <c r="D74" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D75" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="B75" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="3" t="s">
+      <c r="D76" s="7" t="s">
         <v>179</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D77" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="B77" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D77" s="7" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D79" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B80" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B81" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D81" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B82" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>240</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D84" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D85" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="B85" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D86" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="B86" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D86" s="7" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -4387,305 +4384,305 @@
         <v>29</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>83</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>84</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>266</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>188</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="1" t="s">
         <v>211</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>